<commit_message>
PC35 - Added remaining levels up to 15. Added Win screen and new music for it.
</commit_message>
<xml_diff>
--- a/LevelPlan.xlsx
+++ b/LevelPlan.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="30">
   <si>
     <t>Level</t>
   </si>
@@ -68,24 +68,9 @@
     <t>Everything</t>
   </si>
   <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>s</t>
-  </si>
-  <si>
     <t>Cactus + Star</t>
   </si>
   <si>
-    <t>f</t>
-  </si>
-  <si>
-    <t>sn</t>
-  </si>
-  <si>
-    <t>gn</t>
-  </si>
-  <si>
     <t>Spawners</t>
   </si>
   <si>
@@ -126,6 +111,9 @@
   </si>
   <si>
     <t>1,1,1,1,1</t>
+  </si>
+  <si>
+    <t>y</t>
   </si>
 </sst>
 </file>
@@ -452,10 +440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I4"/>
+      <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -465,7 +453,7 @@
     <col min="5" max="5" width="27.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -479,10 +467,10 @@
         <v>3</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -493,38 +481,38 @@
         <v>5</v>
       </c>
       <c r="G2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
       </c>
       <c r="G3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
       </c>
       <c r="G4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -535,10 +523,10 @@
         <v>6</v>
       </c>
       <c r="G5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -555,10 +543,10 @@
         <v>12</v>
       </c>
       <c r="G6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -569,10 +557,10 @@
         <v>6</v>
       </c>
       <c r="G7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -583,10 +571,10 @@
         <v>9</v>
       </c>
       <c r="G8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -600,10 +588,10 @@
         <v>13</v>
       </c>
       <c r="G9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -614,10 +602,10 @@
         <v>9</v>
       </c>
       <c r="G10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -631,57 +619,59 @@
         <v>11</v>
       </c>
       <c r="G11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D12" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="G12" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="G13" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="G14" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
       <c r="G15" t="s">
-        <v>17</v>
-      </c>
-      <c r="H15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16">
         <v>15</v>
       </c>
-      <c r="I15" t="s">
-        <v>14</v>
-      </c>
-      <c r="J15" t="s">
-        <v>18</v>
-      </c>
-      <c r="K15" t="s">
-        <v>19</v>
+      <c r="D16" t="s">
+        <v>29</v>
+      </c>
+      <c r="G16" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>